<commit_message>
GGWP T:N/A S0 - Revisión del backlog y descripción de US
</commit_message>
<xml_diff>
--- a/proyecto/documentos/User Story Mapping (Backlog).xlsx
+++ b/proyecto/documentos/User Story Mapping (Backlog).xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsmaFunes\Documents\Repositories\GitHub\GGWP\proyecto\documentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -15,18 +23,27 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
         <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Significado de colores:
 </t>
     </r>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">Épica
 </t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color rgb="FF38761D"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>Historia de usuario</t>
     </r>
@@ -95,9 +112,6 @@
     <t xml:space="preserve">  Registrar Pago</t>
   </si>
   <si>
-    <t>Registrar Ingreso</t>
-  </si>
-  <si>
     <t>Registrar usuario</t>
   </si>
   <si>
@@ -152,9 +166,6 @@
     <t>Generar pdf comprobante</t>
   </si>
   <si>
-    <t>Registrar Egreso</t>
-  </si>
-  <si>
     <t>Modificar usuario</t>
   </si>
   <si>
@@ -314,43 +325,65 @@
     <t>Generar lista de pagos</t>
   </si>
   <si>
-    <t xml:space="preserve">Asignar actividades a un plan </t>
-  </si>
-  <si>
     <t>Generar lista de socios</t>
+  </si>
+  <si>
+    <t>Registrar Egreso mediante DNI/Legajo</t>
+  </si>
+  <si>
+    <t>Registrar Ingreso mediante DNI/Legajo</t>
+  </si>
+  <si>
+    <t>Imprimir rutina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF38761D"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -366,7 +399,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -380,67 +419,60 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7030A0"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -451,751 +483,1265 @@
           <bgColor rgb="FF38761D"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.29"/>
-    <col customWidth="1" min="2" max="2" width="22.71"/>
-    <col customWidth="1" min="3" max="3" width="23.71"/>
-    <col customWidth="1" min="4" max="4" width="18.71"/>
-    <col customWidth="1" min="5" max="5" width="16.57"/>
-    <col customWidth="1" min="6" max="6" width="14.57"/>
-    <col customWidth="1" min="7" max="7" width="15.29"/>
-    <col customWidth="1" min="8" max="8" width="19.86"/>
-    <col customWidth="1" min="9" max="9" width="16.43"/>
-    <col customWidth="1" min="10" max="10" width="17.71"/>
-    <col customWidth="1" min="11" max="11" width="19.29"/>
-    <col customWidth="1" min="12" max="12" width="17.14"/>
-    <col customWidth="1" min="13" max="13" width="18.0"/>
-    <col customWidth="1" min="14" max="14" width="17.0"/>
-    <col customWidth="1" min="15" max="15" width="14.43"/>
-    <col customWidth="1" min="16" max="16" width="18.0"/>
-    <col customWidth="1" min="17" max="17" width="18.29"/>
-    <col customWidth="1" min="18" max="18" width="17.71"/>
-    <col customWidth="1" min="19" max="19" width="15.86"/>
-    <col customWidth="1" min="20" max="20" width="18.71"/>
-    <col customWidth="1" min="21" max="26" width="10.71"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="21" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" ht="45.75" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" ht="51.0" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+    </row>
+    <row r="2" spans="1:24" ht="51" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" ht="65.25" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="T2" s="8"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+    </row>
+    <row r="3" spans="1:24" ht="65.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="8"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+    </row>
+    <row r="4" spans="1:24" ht="53.25" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-    </row>
-    <row r="4" ht="53.25" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="N4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="P4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="Q4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="R4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="S4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="T4" s="8"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+    </row>
+    <row r="5" spans="1:24" ht="82.5" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-    </row>
-    <row r="5" ht="82.5" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="H5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="N5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="O5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="P5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="Q5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="R5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="S5" s="4"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+    </row>
+    <row r="6" spans="1:24" ht="78" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="S5" s="8"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-    </row>
-    <row r="6" ht="78.0" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="O6" s="5"/>
+      <c r="P6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="6" t="s">
+      <c r="Q6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="6" t="s">
+      <c r="R6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="S6" s="4"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+    </row>
+    <row r="7" spans="1:24" ht="78" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-    </row>
-    <row r="7" ht="78.0" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+    </row>
+    <row r="8" spans="1:24" ht="30.75" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11" t="s">
+      <c r="B8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-    </row>
-    <row r="8" ht="30.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+    </row>
+    <row r="9" spans="1:24" ht="28.5" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="12"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-    </row>
-    <row r="9" ht="28.5" customHeight="1">
-      <c r="A9" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="17"/>
-    </row>
-    <row r="10" ht="27.0" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+    </row>
+    <row r="10" spans="1:24" ht="27" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+    </row>
+    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+    </row>
+    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+    </row>
+    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+    </row>
+    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+    </row>
+    <row r="30" spans="1:24" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:24" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:24" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2166,18 +2712,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="A3:S31 U3:Z31 T9:T31">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:S2 U2:X2">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>